<commit_message>
All csv with aggregated country list now
</commit_message>
<xml_diff>
--- a/SeminarPaper/Model/input data/PotNonDisp.xlsx
+++ b/SeminarPaper/Model/input data/PotNonDisp.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35504ABD-923C-4B30-B62F-7B1D96E483B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C37057-C155-4491-B61B-5974E87BC7FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Potentials Wind and PV</t>
   </si>
@@ -106,6 +106,24 @@
   </si>
   <si>
     <t>PVRoofPot[MW]</t>
+  </si>
+  <si>
+    <t>IB</t>
+  </si>
+  <si>
+    <t>Potentials Wind and PV, Aggregated Country List</t>
+  </si>
+  <si>
+    <t>WindOffshore[MW]</t>
+  </si>
+  <si>
+    <t>WindOnshore[MW]</t>
+  </si>
+  <si>
+    <t>PVGround[MW]</t>
+  </si>
+  <si>
+    <t>PVRoof[MW]</t>
   </si>
 </sst>
 </file>
@@ -241,20 +259,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -270,13 +276,37 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -557,575 +587,739 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:O18"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A4" sqref="A4"/>
+      <selection pane="topRight" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="20"/>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="21"/>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="15" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="31"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="34"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="F4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="G4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="I4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="J4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="K4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="L4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="M4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="22" t="s">
+      <c r="N4" s="16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6">
+      <c r="B5" s="18">
         <v>12.48</v>
       </c>
-      <c r="D5" s="6">
+      <c r="C5" s="18">
         <v>3.18</v>
       </c>
-      <c r="E5" s="8">
+      <c r="D5" s="19">
         <v>15.66</v>
       </c>
-      <c r="F5" s="9">
-        <f>E5/(5*0.001)</f>
+      <c r="E5" s="13">
+        <f>D5/(5*0.001)</f>
         <v>3132</v>
       </c>
-      <c r="G5" s="9">
-        <f>F5*10.76</f>
+      <c r="F5" s="13">
+        <f>E5*10.76</f>
         <v>33700.32</v>
       </c>
-      <c r="H5" s="6">
+      <c r="G5" s="18">
         <v>12</v>
       </c>
-      <c r="I5" s="8">
+      <c r="H5" s="19">
         <v>1714.2857140000001</v>
       </c>
-      <c r="J5" s="8">
-        <f>I5*10.76</f>
+      <c r="I5" s="19">
+        <f>H5*10.76</f>
         <v>18445.714282640001</v>
       </c>
-      <c r="K5" s="6">
+      <c r="J5" s="18">
         <v>3</v>
       </c>
-      <c r="L5" s="8">
+      <c r="K5" s="19">
         <v>19.867549669999999</v>
       </c>
-      <c r="M5" s="6">
-        <f>L5*216.61</f>
+      <c r="L5" s="18">
+        <f>K5*216.61</f>
         <v>4303.5099340186998</v>
       </c>
-      <c r="N5" s="17">
+      <c r="M5" s="13">
         <v>41</v>
       </c>
-      <c r="O5" s="7">
-        <f>N5*216.61</f>
+      <c r="N5" s="20">
+        <f>M5*216.61</f>
         <v>8881.01</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6">
+      <c r="B6" s="2">
         <v>64.44</v>
       </c>
-      <c r="D6" s="6">
+      <c r="C6" s="2">
         <v>163.44999999999999</v>
       </c>
-      <c r="E6" s="8">
+      <c r="D6" s="4">
         <v>227.89</v>
       </c>
-      <c r="F6" s="9">
-        <f t="shared" ref="F6:F13" si="0">E6/(5*0.001)</f>
+      <c r="E6" s="5">
+        <f t="shared" ref="E6:E13" si="0">D6/(5*0.001)</f>
         <v>45577.999999999993</v>
       </c>
-      <c r="G6" s="9">
-        <f t="shared" ref="G6:G13" si="1">F6*10.76</f>
+      <c r="F6" s="5">
+        <f t="shared" ref="F6:F13" si="1">E6*10.76</f>
         <v>490419.27999999991</v>
       </c>
-      <c r="H6" s="6">
+      <c r="G6" s="2">
         <v>24</v>
       </c>
-      <c r="I6" s="8">
+      <c r="H6" s="4">
         <v>3428.5714290000001</v>
       </c>
-      <c r="J6" s="8">
-        <f t="shared" ref="J6:J13" si="2">I6*10.76</f>
+      <c r="I6" s="4">
+        <f t="shared" ref="I6:I13" si="2">H6*10.76</f>
         <v>36891.428576040002</v>
       </c>
-      <c r="K6" s="6">
+      <c r="J6" s="2">
         <v>7</v>
       </c>
-      <c r="L6" s="8">
+      <c r="K6" s="4">
         <v>46.357615889999998</v>
       </c>
-      <c r="M6" s="6">
-        <f t="shared" ref="M6:M13" si="3">L6*216.61</f>
+      <c r="L6" s="2">
+        <f t="shared" ref="L6:L13" si="3">K6*216.61</f>
         <v>10041.523177932901</v>
       </c>
-      <c r="N6" s="17">
+      <c r="M6" s="13">
         <v>63</v>
       </c>
-      <c r="O6" s="7">
-        <f t="shared" ref="O6:O13" si="4">N6*216.61</f>
+      <c r="N6" s="3">
+        <f t="shared" ref="N6:N13" si="4">M6*216.61</f>
         <v>13646.43</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6">
+      <c r="B7" s="2">
         <v>46.42</v>
       </c>
-      <c r="D7" s="6">
+      <c r="C7" s="2">
         <v>134.72</v>
       </c>
-      <c r="E7" s="8">
+      <c r="D7" s="4">
         <v>181.14</v>
       </c>
-      <c r="F7" s="9">
+      <c r="E7" s="5">
         <f t="shared" si="0"/>
         <v>36228</v>
       </c>
-      <c r="G7" s="9">
+      <c r="F7" s="5">
         <f t="shared" si="1"/>
         <v>389813.27999999997</v>
       </c>
-      <c r="H7" s="6">
+      <c r="G7" s="2">
         <v>180</v>
       </c>
-      <c r="I7" s="8">
+      <c r="H7" s="4">
         <v>25714.28571</v>
       </c>
-      <c r="J7" s="8">
+      <c r="I7" s="4">
         <f t="shared" si="2"/>
         <v>276685.7142396</v>
       </c>
-      <c r="K7" s="6">
+      <c r="J7" s="2">
         <v>99</v>
       </c>
-      <c r="L7" s="8">
+      <c r="K7" s="4">
         <v>655.62913909999997</v>
       </c>
-      <c r="M7" s="6">
+      <c r="L7" s="2">
         <f t="shared" si="3"/>
         <v>142015.827820451</v>
       </c>
-      <c r="N7" s="17">
+      <c r="M7" s="13">
         <v>1046</v>
       </c>
-      <c r="O7" s="7">
+      <c r="N7" s="3">
         <f t="shared" si="4"/>
         <v>226574.06000000003</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="6">
+      <c r="B8" s="2">
         <v>27.45</v>
       </c>
-      <c r="D8" s="6">
+      <c r="C8" s="2">
         <v>96.8</v>
       </c>
-      <c r="E8" s="8">
+      <c r="D8" s="4">
         <v>124.25</v>
       </c>
-      <c r="F8" s="9">
+      <c r="E8" s="5">
         <f t="shared" si="0"/>
         <v>24850</v>
       </c>
-      <c r="G8" s="9">
+      <c r="F8" s="5">
         <f t="shared" si="1"/>
         <v>267386</v>
       </c>
-      <c r="H8" s="6">
+      <c r="G8" s="2">
         <v>110</v>
       </c>
-      <c r="I8" s="8">
+      <c r="H8" s="4">
         <v>15714.28571</v>
       </c>
-      <c r="J8" s="8">
+      <c r="I8" s="4">
         <f t="shared" si="2"/>
         <v>169085.7142396</v>
       </c>
-      <c r="K8" s="6">
+      <c r="J8" s="2">
         <v>39</v>
       </c>
-      <c r="L8" s="8">
+      <c r="K8" s="4">
         <v>258.27814569999998</v>
       </c>
-      <c r="M8" s="6">
+      <c r="L8" s="2">
         <f t="shared" si="3"/>
         <v>55945.629140076999</v>
       </c>
-      <c r="N8" s="17">
+      <c r="M8" s="13">
         <v>952</v>
       </c>
-      <c r="O8" s="7">
+      <c r="N8" s="3">
         <f t="shared" si="4"/>
         <v>206212.72</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="5" t="s">
+    <row r="9" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="6">
+      <c r="B9" s="18">
         <v>0</v>
       </c>
-      <c r="D9" s="6">
+      <c r="C9" s="18">
         <v>0</v>
       </c>
-      <c r="E9" s="8">
+      <c r="D9" s="19">
         <v>0</v>
       </c>
-      <c r="F9" s="9">
+      <c r="E9" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="9">
+      <c r="F9" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H9" s="6">
+      <c r="G9" s="18">
         <v>1</v>
       </c>
-      <c r="I9" s="8">
+      <c r="H9" s="19">
         <v>142.85714290000001</v>
       </c>
-      <c r="J9" s="8">
+      <c r="I9" s="19">
         <f t="shared" si="2"/>
         <v>1537.142857604</v>
       </c>
-      <c r="K9" s="6">
+      <c r="J9" s="18">
         <v>0</v>
       </c>
-      <c r="L9" s="8">
+      <c r="K9" s="19">
         <v>0</v>
       </c>
-      <c r="M9" s="6">
+      <c r="L9" s="18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N9" s="17">
+      <c r="M9" s="13">
         <v>4</v>
       </c>
-      <c r="O9" s="7">
+      <c r="N9" s="20">
         <f t="shared" si="4"/>
         <v>866.44</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="6">
+      <c r="B10" s="18">
         <v>110.14</v>
       </c>
-      <c r="D10" s="6">
+      <c r="C10" s="18">
         <v>150.9</v>
       </c>
-      <c r="E10" s="8">
+      <c r="D10" s="19">
         <v>261.04000000000002</v>
       </c>
-      <c r="F10" s="9">
+      <c r="E10" s="13">
         <f t="shared" si="0"/>
         <v>52208</v>
       </c>
-      <c r="G10" s="9">
+      <c r="F10" s="13">
         <f t="shared" si="1"/>
         <v>561758.07999999996</v>
       </c>
-      <c r="H10" s="6">
+      <c r="G10" s="18">
         <v>18</v>
       </c>
-      <c r="I10" s="8">
+      <c r="H10" s="19">
         <v>2571.4285709999999</v>
       </c>
-      <c r="J10" s="8">
+      <c r="I10" s="19">
         <f t="shared" si="2"/>
         <v>27668.571423959998</v>
       </c>
-      <c r="K10" s="6">
+      <c r="J10" s="18">
         <v>6</v>
       </c>
-      <c r="L10" s="8">
+      <c r="K10" s="19">
         <v>39.735099339999998</v>
       </c>
-      <c r="M10" s="6">
+      <c r="L10" s="18">
         <f t="shared" si="3"/>
         <v>8607.0198680373996</v>
       </c>
-      <c r="N10" s="17">
+      <c r="M10" s="13">
         <v>75</v>
       </c>
-      <c r="O10" s="7">
+      <c r="N10" s="20">
         <f t="shared" si="4"/>
         <v>16245.750000000002</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="5" t="s">
+    <row r="11" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="6">
+      <c r="B11" s="23">
         <v>0.66</v>
       </c>
-      <c r="D11" s="6">
+      <c r="C11" s="23">
         <v>11.32</v>
       </c>
-      <c r="E11" s="8">
+      <c r="D11" s="24">
         <v>11.98</v>
       </c>
-      <c r="F11" s="9">
+      <c r="E11" s="25">
         <f t="shared" si="0"/>
         <v>2396</v>
       </c>
-      <c r="G11" s="9">
+      <c r="F11" s="25">
         <f t="shared" si="1"/>
         <v>25780.959999999999</v>
       </c>
-      <c r="H11" s="6">
+      <c r="G11" s="23">
         <v>10</v>
       </c>
-      <c r="I11" s="8">
+      <c r="H11" s="24">
         <v>1428.5714290000001</v>
       </c>
-      <c r="J11" s="8">
+      <c r="I11" s="24">
         <f t="shared" si="2"/>
         <v>15371.42857604</v>
       </c>
-      <c r="K11" s="6">
+      <c r="J11" s="23">
         <v>19</v>
       </c>
-      <c r="L11" s="8">
+      <c r="K11" s="24">
         <v>125.8278146</v>
       </c>
-      <c r="M11" s="6">
+      <c r="L11" s="23">
         <f t="shared" si="3"/>
         <v>27255.562920506</v>
       </c>
-      <c r="N11" s="17">
+      <c r="M11" s="26">
         <v>211</v>
       </c>
-      <c r="O11" s="7">
+      <c r="N11" s="27">
         <f t="shared" si="4"/>
         <v>45704.710000000006</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="5" t="s">
+    <row r="12" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="6">
+      <c r="B12" s="23">
         <v>21.36</v>
       </c>
-      <c r="D12" s="6">
+      <c r="C12" s="23">
         <v>9.92</v>
       </c>
-      <c r="E12" s="8">
+      <c r="D12" s="24">
         <v>31.28</v>
       </c>
-      <c r="F12" s="9">
-        <f>E12/(5*0.001)</f>
+      <c r="E12" s="25">
+        <f>D12/(5*0.001)</f>
         <v>6256</v>
       </c>
-      <c r="G12" s="9">
+      <c r="F12" s="25">
         <f t="shared" si="1"/>
         <v>67314.559999999998</v>
       </c>
-      <c r="H12" s="6">
+      <c r="G12" s="23">
         <v>71</v>
       </c>
-      <c r="I12" s="8">
+      <c r="H12" s="24">
         <v>10142.85714</v>
       </c>
-      <c r="J12" s="8">
+      <c r="I12" s="24">
         <f t="shared" si="2"/>
         <v>109137.1428264</v>
       </c>
-      <c r="K12" s="6">
+      <c r="J12" s="23">
         <v>137</v>
       </c>
-      <c r="L12" s="8">
+      <c r="K12" s="24">
         <v>907.28476820000003</v>
       </c>
-      <c r="M12" s="6">
+      <c r="L12" s="23">
         <f t="shared" si="3"/>
         <v>196526.95363980203</v>
       </c>
-      <c r="N12" s="17">
+      <c r="M12" s="26">
         <v>823</v>
       </c>
-      <c r="O12" s="7">
+      <c r="N12" s="27">
         <f t="shared" si="4"/>
         <v>178270.03</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="10" t="s">
+    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="11">
+      <c r="B13" s="7">
         <v>167.48</v>
       </c>
-      <c r="D13" s="11">
+      <c r="C13" s="7">
         <v>463.76</v>
       </c>
-      <c r="E13" s="12">
+      <c r="D13" s="8">
         <v>631.24</v>
       </c>
-      <c r="F13" s="13">
+      <c r="E13" s="9">
         <f t="shared" si="0"/>
         <v>126248</v>
       </c>
-      <c r="G13" s="13">
+      <c r="F13" s="9">
         <f t="shared" si="1"/>
         <v>1358428.48</v>
       </c>
-      <c r="H13" s="11">
+      <c r="G13" s="7">
         <v>127</v>
       </c>
-      <c r="I13" s="12">
+      <c r="H13" s="8">
         <v>18142.85714</v>
       </c>
-      <c r="J13" s="12">
+      <c r="I13" s="8">
         <f t="shared" si="2"/>
         <v>195217.1428264</v>
       </c>
-      <c r="K13" s="11">
+      <c r="J13" s="7">
         <v>147</v>
       </c>
-      <c r="L13" s="12">
+      <c r="K13" s="8">
         <v>973.5099338</v>
       </c>
-      <c r="M13" s="11">
+      <c r="L13" s="7">
         <f t="shared" si="3"/>
         <v>210871.98676041802</v>
       </c>
-      <c r="N13" s="18">
+      <c r="M13" s="14">
         <v>530</v>
       </c>
-      <c r="O13" s="19">
+      <c r="N13" s="15">
         <f t="shared" si="4"/>
         <v>114803.3</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B16" s="16" t="s">
+    <row r="14" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="16" t="s">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="16" t="s">
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-    </row>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="31"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="32"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="34"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="5">
+        <f>F6</f>
+        <v>490419.27999999991</v>
+      </c>
+      <c r="D23" s="4">
+        <f>I6</f>
+        <v>36891.428576040002</v>
+      </c>
+      <c r="E23" s="2">
+        <f>L6</f>
+        <v>10041.523177932901</v>
+      </c>
+      <c r="F23" s="3">
+        <f>N6</f>
+        <v>13646.43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="5">
+        <f>F7</f>
+        <v>389813.27999999997</v>
+      </c>
+      <c r="D24" s="4">
+        <f>I7</f>
+        <v>276685.7142396</v>
+      </c>
+      <c r="E24" s="2">
+        <f>L7</f>
+        <v>142015.827820451</v>
+      </c>
+      <c r="F24" s="3">
+        <f>N7</f>
+        <v>226574.06000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="5">
+        <f>F8</f>
+        <v>267386</v>
+      </c>
+      <c r="D25" s="4">
+        <f>I8</f>
+        <v>169085.7142396</v>
+      </c>
+      <c r="E25" s="2">
+        <f>L8</f>
+        <v>55945.629140076999</v>
+      </c>
+      <c r="F25" s="3">
+        <f>N8</f>
+        <v>206212.72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="5">
+        <f>F5+F9+F10</f>
+        <v>595458.39999999991</v>
+      </c>
+      <c r="D26" s="4">
+        <f>I5+I9+I10</f>
+        <v>47651.428564204005</v>
+      </c>
+      <c r="E26" s="2">
+        <f>L5+L9+L10</f>
+        <v>12910.529802056099</v>
+      </c>
+      <c r="F26" s="3">
+        <f>N5+N9+N10</f>
+        <v>25993.200000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="5">
+        <f>F11+F12</f>
+        <v>93095.51999999999</v>
+      </c>
+      <c r="D27" s="4">
+        <f>I11+I12</f>
+        <v>124508.57140243999</v>
+      </c>
+      <c r="E27" s="2">
+        <f>L11+L12</f>
+        <v>223782.51656030802</v>
+      </c>
+      <c r="F27" s="3">
+        <f>N11+N12</f>
+        <v>223974.74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="9">
+        <f>F13</f>
+        <v>1358428.48</v>
+      </c>
+      <c r="D28" s="8">
+        <f>I13</f>
+        <v>195217.1428264</v>
+      </c>
+      <c r="E28" s="7">
+        <f>L13</f>
+        <v>210871.98676041802</v>
+      </c>
+      <c r="F28" s="15">
+        <f>N13</f>
+        <v>114803.3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:O3"/>
+  <mergeCells count="2">
+    <mergeCell ref="A2:N3"/>
+    <mergeCell ref="B20:F21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>